<commit_message>
Change to correct covidence ID for KM's paper
</commit_message>
<xml_diff>
--- a/data/marburg/raw/marburg_article.xlsx
+++ b/data/marburg/raw/marburg_article.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc4018\Documents\code\priority-pathogens\src\data_cleaning\data\marburg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kem22_ic_ac_uk/Documents/Projects/Priority Pathogens/priority-pathogens/data/marburg/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13AF751F-8B6A-43D5-983A-264401CEAA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{13AF751F-8B6A-43D5-983A-264401CEAA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C29E665B-0E36-4541-9FF6-509E24285568}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="14292" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Article data - Table" sheetId="1" r:id="rId1"/>
@@ -1328,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1668,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="2">
-        <v>1962</v>
+        <v>1692</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>49</v>

</xml_diff>